<commit_message>
Replace excel file with new test cases
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#VITALSOFTWAREXX/VitalSoftware/Isolab9002/2.0/accreditamento-checklist_V8.2.5.xlsx
+++ b/GATEWAY/A1#111#VITALSOFTWAREXX/VitalSoftware/Isolab9002/2.0/accreditamento-checklist_V8.2.5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaa\progEst\VitalSW_RicetteElettroniche_FSE2\20241210_docs\0_Accreditamento\docs_per_accreditamento\VitalSW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaa\progEst\VitalSW_RicetteElettroniche_FSE2\20241210_docs\0_Accreditamento\docs_per_accreditamento\A1#111#VITALSOFTWAREXX\VitalSoftware\Isolab9002\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603A2530-D3E4-4549-9856-C7BF23B6A304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A89DF25-85D0-4907-970B-670140BBCF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1950" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$26</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,9 +39,6 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="oXWj5iU3LtnvLpdhFqszSz/X91q3fG5U5zC5TJKtiGw="/>
     </ext>
   </extLst>
 </workbook>
@@ -80,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="185">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -772,6 +769,43 @@
   <si>
     <t>Vitale Salvatore</t>
   </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST- OK" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST OK - HLA" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>28/5/2025</t>
+  </si>
+  <si>
+    <t>18:16:56</t>
+  </si>
+  <si>
+    <t>18:17:25</t>
+  </si>
+  <si>
+    <t>0e8e1596e30e6c882112fa1b009e887b</t>
+  </si>
+  <si>
+    <t>ff595c895e66c26bff1989a4b7f65cc3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a2aea048da11324375f7e287c382a58f0c76be29f8bba948511b240dca9b6999.dbf5077ca9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a2aea048da11324375f7e287c382a58f0c76be29f8bba948511b240dca9b6999.e1d28a58fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
 </sst>
 </file>
 
@@ -780,11 +814,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1243,174 +1284,221 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{565105C8-FFD6-432C-8B2E-BD1D172FCD26}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{527C9706-56CA-4FEA-B7CA-BF499827724E}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2849,13 +2937,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W587"/>
+  <dimension ref="A1:W589"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="R10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3:D3"/>
+      <selection pane="bottomRight" activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3944,156 +4032,214 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="35">
+      <c r="A23" s="69">
+        <v>191</v>
+      </c>
+      <c r="B23" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="69" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="77" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="I23" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="J23" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="72"/>
+      <c r="S23" s="72"/>
+      <c r="T23" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="U23" s="73"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="72" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="63">
+        <v>376</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="E24" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="I24" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="J24" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="U24" s="65"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35">
         <v>452</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B25" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C25" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D25" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E25" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="36" t="s">
+      <c r="F25" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G25" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="H23" s="37" t="s">
+      <c r="H25" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="I23" s="42" t="s">
+      <c r="I25" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="J23" s="38" t="s">
+      <c r="J25" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38" t="s">
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="U23" s="39"/>
-      <c r="V23" s="40"/>
-      <c r="W23" s="38" t="s">
+      <c r="U25" s="39"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35">
+    <row r="26" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35">
         <v>466</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B26" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C26" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D26" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E26" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="36" t="s">
+      <c r="F26" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="G24" s="48" t="s">
+      <c r="G26" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H26" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="I24" s="49" t="s">
+      <c r="I26" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J26" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="38"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="38" t="s">
+      <c r="K26" s="38"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="N24" s="38" t="s">
+      <c r="N26" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="O24" s="35" t="s">
+      <c r="O26" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="P24" s="38" t="s">
+      <c r="P26" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="Q24" s="38" t="s">
+      <c r="Q26" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="R24" s="38" t="s">
+      <c r="R26" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="S24" s="38" t="s">
+      <c r="S26" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="T24" s="38" t="s">
+      <c r="T26" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35" t="s">
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="6"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="9"/>
-    </row>
-    <row r="26" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="6"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="9"/>
     </row>
     <row r="27" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="6"/>
@@ -6876,10 +7022,44 @@
       <c r="W165" s="9"/>
     </row>
     <row r="166" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="W166" s="7"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="45"/>
+      <c r="H166" s="6"/>
+      <c r="I166" s="6"/>
+      <c r="J166" s="7"/>
+      <c r="K166" s="7"/>
+      <c r="L166" s="7"/>
+      <c r="M166" s="7"/>
+      <c r="N166" s="7"/>
+      <c r="O166" s="7"/>
+      <c r="P166" s="7"/>
+      <c r="Q166" s="7"/>
+      <c r="R166" s="7"/>
+      <c r="S166" s="7"/>
+      <c r="T166" s="7"/>
+      <c r="U166" s="8"/>
+      <c r="V166" s="2"/>
+      <c r="W166" s="9"/>
     </row>
     <row r="167" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="W167" s="7"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="45"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+      <c r="J167" s="7"/>
+      <c r="K167" s="7"/>
+      <c r="L167" s="7"/>
+      <c r="M167" s="7"/>
+      <c r="N167" s="7"/>
+      <c r="O167" s="7"/>
+      <c r="P167" s="7"/>
+      <c r="Q167" s="7"/>
+      <c r="R167" s="7"/>
+      <c r="S167" s="7"/>
+      <c r="T167" s="7"/>
+      <c r="U167" s="8"/>
+      <c r="V167" s="2"/>
+      <c r="W167" s="9"/>
     </row>
     <row r="168" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W168" s="7"/>
@@ -8126,13 +8306,19 @@
     <row r="582" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W582" s="7"/>
     </row>
-    <row r="583" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W583" s="7"/>
+    </row>
+    <row r="584" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W584" s="7"/>
+    </row>
     <row r="585" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="586" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="587" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W24" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W26" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -8142,7 +8328,7 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -8153,19 +8339,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M10:N24 J10:J24 P10:R24</xm:sqref>
+          <xm:sqref>M10:N26 J10:J26 P10:R26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T10:T24</xm:sqref>
+          <xm:sqref>T10:T26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K24</xm:sqref>
+          <xm:sqref>K10:K26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10416,18 +10602,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10685,6 +10859,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10695,23 +10881,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10730,6 +10899,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>

</xml_diff>